<commit_message>
Modify readRowsFromSheet to handle series of rows and cells omitted from the XML because they're blank.
</commit_message>
<xml_diff>
--- a/wpsBlankLineTest.xlsx
+++ b/wpsBlankLineTest.xlsx
@@ -436,12 +436,14 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>
+        0</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>
+        0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>